<commit_message>
create_abstract end point added
</commit_message>
<xml_diff>
--- a/bill docs/22SNCJO-373/attendance/attendance_format_2_2024.xlsx
+++ b/bill docs/22SNCJO-373/attendance/attendance_format_2_2024.xlsx
@@ -3752,7 +3752,7 @@
         <v>138.26</v>
       </c>
       <c r="K6" s="357" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L6" s="357" t="n">
         <v>1938.26</v>
@@ -3773,7 +3773,7 @@
         <v>2549.1</v>
       </c>
       <c r="R6" s="357" t="n">
-        <v>16345.74</v>
+        <v>16495.74</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1" s="339">
@@ -3806,7 +3806,7 @@
         <v>138.26</v>
       </c>
       <c r="K7" s="359" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L7" s="359" t="n">
         <v>1938.26</v>
@@ -3827,7 +3827,7 @@
         <v>2549.1</v>
       </c>
       <c r="R7" s="359" t="n">
-        <v>16345.74</v>
+        <v>16495.74</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1" s="339">
@@ -3864,7 +3864,7 @@
         <v>112.65</v>
       </c>
       <c r="K8" s="357" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L8" s="357" t="n">
         <v>1912.65</v>
@@ -3885,7 +3885,7 @@
         <v>2438.13</v>
       </c>
       <c r="R8" s="357" t="n">
-        <v>12956.85</v>
+        <v>13106.85</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1" s="339">
@@ -3918,7 +3918,7 @@
         <v>112.65</v>
       </c>
       <c r="K9" s="359" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L9" s="359" t="n">
         <v>1912.65</v>
@@ -3939,7 +3939,7 @@
         <v>2438.13</v>
       </c>
       <c r="R9" s="359" t="n">
-        <v>12956.85</v>
+        <v>13106.85</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1" s="339">
@@ -4084,7 +4084,7 @@
         <v>343.52</v>
       </c>
       <c r="K12" s="362" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="L12" s="362" t="n">
         <v>5425.28</v>
@@ -4105,7 +4105,7 @@
         <v>6993.78</v>
       </c>
       <c r="R12" s="362" t="n">
-        <v>40076.22</v>
+        <v>40376.22</v>
       </c>
     </row>
     <row r="16">

</xml_diff>